<commit_message>
Reaction wheels and meeting minutes
</commit_message>
<xml_diff>
--- a/Alex/Reaction Wheels/Reaction Wheels.xlsx
+++ b/Alex/Reaction Wheels/Reaction Wheels.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\CubeSat_project\Alex\Reaction Wheels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48E24C1-08E6-4DAF-9B73-5A973936CF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081FD759-2DF9-46A2-8C7C-9C9D8F44B4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>Company</t>
   </si>
@@ -75,20 +86,77 @@
     <t>Max Torque Power (W)</t>
   </si>
   <si>
-    <t>Supply voltage (V)</t>
-  </si>
-  <si>
     <t>Max voltage (V)</t>
   </si>
   <si>
     <t>Min voltage (V)</t>
+  </si>
+  <si>
+    <t>Max 8U rotational speed (rads-1)</t>
+  </si>
+  <si>
+    <t>Max 8U rotational speeds (rpm)</t>
+  </si>
+  <si>
+    <t>Space Inventor</t>
+  </si>
+  <si>
+    <t>WHL-1000</t>
+  </si>
+  <si>
+    <t>https://satsearch.co/products/space-inventor-whl-1000</t>
+  </si>
+  <si>
+    <t>RW400</t>
+  </si>
+  <si>
+    <t>AA Clyde Space</t>
+  </si>
+  <si>
+    <t>RW401</t>
+  </si>
+  <si>
+    <t>RW402</t>
+  </si>
+  <si>
+    <t>GranStal</t>
+  </si>
+  <si>
+    <t>GS-RWT37</t>
+  </si>
+  <si>
+    <t>GS-RWT41</t>
+  </si>
+  <si>
+    <t>GS-RWS15</t>
+  </si>
+  <si>
+    <t>GS-RWS56</t>
+  </si>
+  <si>
+    <t>GS-RWS67</t>
+  </si>
+  <si>
+    <t>GS-RW10</t>
+  </si>
+  <si>
+    <t>GS-RW60</t>
+  </si>
+  <si>
+    <t>GS-RW200</t>
+  </si>
+  <si>
+    <t>GS-RW400</t>
+  </si>
+  <si>
+    <t>Steady voltage (V)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,13 +172,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -122,14 +210,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -408,14 +503,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="17.140625" customWidth="1"/>
@@ -426,9 +523,11 @@
     <col min="13" max="13" width="15.5703125" customWidth="1"/>
     <col min="14" max="14" width="16.42578125" customWidth="1"/>
     <col min="15" max="15" width="16.7109375" customWidth="1"/>
+    <col min="16" max="16" width="32.85546875" customWidth="1"/>
+    <col min="17" max="17" width="33.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,16 +565,22 @@
         <v>15</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -521,8 +626,16 @@
       <c r="O2">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2">
+        <f>F2*0.001</f>
+        <v>0.02</v>
+      </c>
+      <c r="Q2" s="3">
+        <f>(P2/(2*PI())*60)</f>
+        <v>0.19098593171027442</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -568,8 +681,16 @@
       <c r="O3">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <f>F3*0.001</f>
+        <v>0.04</v>
+      </c>
+      <c r="Q3" s="3">
+        <f t="shared" ref="Q3:Q17" si="0">(P3/(2*PI())*60)</f>
+        <v>0.38197186342054884</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -615,8 +736,638 @@
       <c r="O4">
         <v>18</v>
       </c>
+      <c r="P4">
+        <f>F4*0.001</f>
+        <v>0.06</v>
+      </c>
+      <c r="Q4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.57295779513082312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>109</v>
+      </c>
+      <c r="D5">
+        <v>109</v>
+      </c>
+      <c r="E5">
+        <v>42.5</v>
+      </c>
+      <c r="F5">
+        <v>1000</v>
+      </c>
+      <c r="G5">
+        <v>50</v>
+      </c>
+      <c r="H5">
+        <v>8100</v>
+      </c>
+      <c r="J5">
+        <v>1200</v>
+      </c>
+      <c r="K5">
+        <v>9</v>
+      </c>
+      <c r="L5">
+        <v>44</v>
+      </c>
+      <c r="O5">
+        <v>28</v>
+      </c>
+      <c r="P5">
+        <f>F5*0.001</f>
+        <v>1</v>
+      </c>
+      <c r="Q5" s="3">
+        <f t="shared" si="0"/>
+        <v>9.5492965855137211</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+      <c r="E6">
+        <v>27</v>
+      </c>
+      <c r="F6">
+        <v>15</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>5000</v>
+      </c>
+      <c r="J6">
+        <v>197</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>15</v>
+      </c>
+      <c r="M6">
+        <v>4.5</v>
+      </c>
+      <c r="N6">
+        <v>5</v>
+      </c>
+      <c r="O6">
+        <v>0.5</v>
+      </c>
+      <c r="P6">
+        <f>F6*0.001</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Q6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.14323944878270578</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>50</v>
+      </c>
+      <c r="E7">
+        <v>27</v>
+      </c>
+      <c r="F7">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>5000</v>
+      </c>
+      <c r="J7">
+        <v>210</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>15</v>
+      </c>
+      <c r="M7">
+        <v>4.5</v>
+      </c>
+      <c r="N7">
+        <v>5</v>
+      </c>
+      <c r="O7">
+        <v>0.5</v>
+      </c>
+      <c r="P7">
+        <f>F7*0.001</f>
+        <v>0.03</v>
+      </c>
+      <c r="Q7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.28647889756541156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>27</v>
+      </c>
+      <c r="F8">
+        <v>50</v>
+      </c>
+      <c r="G8">
+        <v>8</v>
+      </c>
+      <c r="H8">
+        <v>5000</v>
+      </c>
+      <c r="J8">
+        <v>375</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>15</v>
+      </c>
+      <c r="M8">
+        <v>4.5</v>
+      </c>
+      <c r="N8">
+        <v>5</v>
+      </c>
+      <c r="O8">
+        <v>0.5</v>
+      </c>
+      <c r="P8">
+        <f>F8*0.001</f>
+        <v>0.05</v>
+      </c>
+      <c r="Q8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.47746482927568601</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>37</v>
+      </c>
+      <c r="D9">
+        <v>37</v>
+      </c>
+      <c r="E9">
+        <v>37</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>0.45</v>
+      </c>
+      <c r="H9">
+        <v>6000</v>
+      </c>
+      <c r="J9">
+        <v>90</v>
+      </c>
+      <c r="K9">
+        <v>0.7</v>
+      </c>
+      <c r="L9">
+        <v>2.5</v>
+      </c>
+      <c r="N9">
+        <v>8</v>
+      </c>
+      <c r="P9">
+        <f>F9*0.001</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="Q9" s="3">
+        <f t="shared" si="0"/>
+        <v>2.8647889756541162E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>41</v>
+      </c>
+      <c r="D10">
+        <v>41</v>
+      </c>
+      <c r="E10">
+        <v>41</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <v>0.45</v>
+      </c>
+      <c r="H10">
+        <v>8000</v>
+      </c>
+      <c r="J10">
+        <v>115</v>
+      </c>
+      <c r="K10">
+        <v>0.8</v>
+      </c>
+      <c r="L10">
+        <v>2.5</v>
+      </c>
+      <c r="N10">
+        <v>8</v>
+      </c>
+      <c r="P10">
+        <f t="shared" ref="P10:P17" si="1">F10*0.001</f>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="Q10" s="3">
+        <f>(P10/(2*PI())*60)</f>
+        <v>5.7295779513082325E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>49</v>
+      </c>
+      <c r="D11">
+        <v>49</v>
+      </c>
+      <c r="E11">
+        <v>23</v>
+      </c>
+      <c r="F11">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>2.5</v>
+      </c>
+      <c r="H11">
+        <v>6500</v>
+      </c>
+      <c r="J11">
+        <v>150</v>
+      </c>
+      <c r="K11">
+        <v>2.5</v>
+      </c>
+      <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="N11">
+        <v>8</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="1"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Q11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.14323944878270578</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12">
+        <v>49</v>
+      </c>
+      <c r="D12">
+        <v>49</v>
+      </c>
+      <c r="E12">
+        <v>49</v>
+      </c>
+      <c r="F12">
+        <v>56</v>
+      </c>
+      <c r="G12">
+        <v>8</v>
+      </c>
+      <c r="H12">
+        <v>6200</v>
+      </c>
+      <c r="J12">
+        <v>460</v>
+      </c>
+      <c r="K12">
+        <v>2.5</v>
+      </c>
+      <c r="L12">
+        <v>7.5</v>
+      </c>
+      <c r="N12">
+        <v>8</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="1"/>
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="Q12" s="3">
+        <f>(P12/(2*PI())*60)</f>
+        <v>0.5347606087887683</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>70</v>
+      </c>
+      <c r="D13">
+        <v>70</v>
+      </c>
+      <c r="E13">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="F13">
+        <v>67</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>6500</v>
+      </c>
+      <c r="J13">
+        <v>450</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+      <c r="L13">
+        <v>7.5</v>
+      </c>
+      <c r="N13">
+        <v>8</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="1"/>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="Q13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.63980287122941937</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="5">
+        <v>50</v>
+      </c>
+      <c r="D14" s="5">
+        <v>50</v>
+      </c>
+      <c r="E14" s="5">
+        <v>60</v>
+      </c>
+      <c r="F14" s="5">
+        <v>100</v>
+      </c>
+      <c r="G14" s="5">
+        <v>10</v>
+      </c>
+      <c r="H14" s="5">
+        <v>6800</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5">
+        <v>250</v>
+      </c>
+      <c r="K14" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="Q14" s="6">
+        <f t="shared" si="0"/>
+        <v>0.95492965855137202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15">
+        <v>100</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15">
+        <v>65</v>
+      </c>
+      <c r="F15">
+        <v>600</v>
+      </c>
+      <c r="G15">
+        <v>20</v>
+      </c>
+      <c r="H15">
+        <v>6500</v>
+      </c>
+      <c r="J15">
+        <v>1050</v>
+      </c>
+      <c r="K15">
+        <v>4.5</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="Q15" s="3">
+        <f t="shared" si="0"/>
+        <v>5.7295779513082321</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16">
+        <v>130</v>
+      </c>
+      <c r="D16">
+        <v>130</v>
+      </c>
+      <c r="E16">
+        <v>85</v>
+      </c>
+      <c r="F16">
+        <v>2000</v>
+      </c>
+      <c r="G16">
+        <v>60</v>
+      </c>
+      <c r="H16">
+        <v>6200</v>
+      </c>
+      <c r="J16">
+        <v>1850</v>
+      </c>
+      <c r="K16">
+        <v>5</v>
+      </c>
+      <c r="M16">
+        <v>20</v>
+      </c>
+      <c r="N16">
+        <v>28</v>
+      </c>
+      <c r="O16">
+        <v>32</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="Q16" s="3">
+        <f t="shared" si="0"/>
+        <v>19.098593171027442</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17">
+        <v>170</v>
+      </c>
+      <c r="D17">
+        <v>170</v>
+      </c>
+      <c r="E17">
+        <v>91</v>
+      </c>
+      <c r="F17">
+        <v>4000</v>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+      <c r="H17">
+        <v>5600</v>
+      </c>
+      <c r="J17">
+        <v>280</v>
+      </c>
+      <c r="K17">
+        <v>10</v>
+      </c>
+      <c r="M17">
+        <v>20</v>
+      </c>
+      <c r="N17">
+        <v>28</v>
+      </c>
+      <c r="O17">
+        <v>32</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Q17" s="3">
+        <f t="shared" si="0"/>
+        <v>38.197186342054884</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="R5" r:id="rId1" xr:uid="{75F5C08A-549C-4A85-AA18-36A54A2F83F0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>